<commit_message>
Adds more tests and fixtures
</commit_message>
<xml_diff>
--- a/tests/fixtures/test.xlsx
+++ b/tests/fixtures/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattj_000\Documents\GitHub\trapp\tests\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjbernha\Documents\GitHub\trapp\tests\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -353,7 +353,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>